<commit_message>
completed the rest of the operations
</commit_message>
<xml_diff>
--- a/Test_Data/TestData.xlsx
+++ b/Test_Data/TestData.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\easwarsa\workspace\RestAPI_Test1\Test_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seaswaran2\eclipse-workspace\REST_API_Testing\Test_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7782315-AD8F-4593-B0D8-7967648308B0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="6570"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="6570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Post" sheetId="1" r:id="rId1"/>
+    <sheet name="Booking" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="47">
   <si>
     <t>Yes</t>
   </si>
@@ -27,70 +28,145 @@
     <t>Execute</t>
   </si>
   <si>
-    <t>book_name</t>
-  </si>
-  <si>
-    <t>isbn</t>
-  </si>
-  <si>
-    <t>aisle</t>
-  </si>
-  <si>
-    <t>author</t>
-  </si>
-  <si>
-    <t>Futuristic1</t>
-  </si>
-  <si>
-    <t>fute1</t>
-  </si>
-  <si>
-    <t>111</t>
-  </si>
-  <si>
-    <t>Yuval Harari</t>
-  </si>
-  <si>
-    <t>Futuristic2</t>
-  </si>
-  <si>
-    <t>Futuristic3</t>
-  </si>
-  <si>
-    <t>Futuristic4</t>
-  </si>
-  <si>
-    <t>fute2</t>
-  </si>
-  <si>
-    <t>fute3</t>
-  </si>
-  <si>
-    <t>fute4</t>
-  </si>
-  <si>
     <t>112</t>
   </si>
   <si>
-    <t>113</t>
-  </si>
-  <si>
-    <t>114</t>
-  </si>
-  <si>
     <t>Test case</t>
   </si>
   <si>
-    <t>Post_testingFromDataFile</t>
-  </si>
-  <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>firstname</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>totalprice</t>
+  </si>
+  <si>
+    <t>depositpaid</t>
+  </si>
+  <si>
+    <t>checkin</t>
+  </si>
+  <si>
+    <t>checkout</t>
+  </si>
+  <si>
+    <t>additionalneeds</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Mary</t>
+  </si>
+  <si>
+    <t>Jackson</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>Breakfast</t>
+  </si>
+  <si>
+    <t>Sally</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>816</t>
+  </si>
+  <si>
+    <t>2019-03-29</t>
+  </si>
+  <si>
+    <t>2019-04-21</t>
+  </si>
+  <si>
+    <t>Susan</t>
+  </si>
+  <si>
+    <t>916</t>
+  </si>
+  <si>
+    <t>2017-04-04</t>
+  </si>
+  <si>
+    <t>2018-06-13</t>
+  </si>
+  <si>
+    <t>Jones</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>712</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>2015-05-04</t>
+  </si>
+  <si>
+    <t>2019-04-02</t>
+  </si>
+  <si>
+    <t>Marie</t>
+  </si>
+  <si>
+    <t>EndRow</t>
+  </si>
+  <si>
+    <t>243</t>
+  </si>
+  <si>
+    <t>2017-04-16</t>
+  </si>
+  <si>
+    <t>2018-02-03</t>
+  </si>
+  <si>
+    <t>GetBooking</t>
+  </si>
+  <si>
+    <t>CreateBooking</t>
+  </si>
+  <si>
+    <t>Lunch</t>
+  </si>
+  <si>
+    <t>Jimmy</t>
+  </si>
+  <si>
+    <t>Browny</t>
+  </si>
+  <si>
+    <t>2017-01-02</t>
+  </si>
+  <si>
+    <t>2017-01-30</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -107,7 +183,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -123,6 +199,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -154,7 +236,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -176,6 +258,12 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -524,124 +612,260 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="24.85546875" style="5" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" customWidth="1"/>
-    <col min="15" max="15" width="19.140625" customWidth="1"/>
-    <col min="16" max="16" width="16.140625" customWidth="1"/>
-    <col min="22" max="22" width="15.42578125" customWidth="1"/>
-    <col min="23" max="23" width="18.85546875" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="5" max="7" width="13" style="5" customWidth="1"/>
+    <col min="8" max="8" width="13" customWidth="1"/>
+    <col min="9" max="10" width="13" style="5" customWidth="1"/>
+    <col min="14" max="14" width="19.140625" customWidth="1"/>
+    <col min="15" max="15" width="16.140625" customWidth="1"/>
+    <col min="21" max="21" width="15.42578125" customWidth="1"/>
+    <col min="22" max="22" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>5</v>
+        <v>8</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>9</v>
+        <v>37</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" s="4"/>
+      <c r="K2" s="9" t="s">
+        <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>13</v>
-      </c>
       <c r="E3" s="4" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>9</v>
+        <v>22</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="J5" s="4"/>
+      <c r="K5" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="7" t="s">
         <v>9</v>
       </c>
+      <c r="G6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="5" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="3" t="s">
+    <row r="7" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>9</v>
+      <c r="C7" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>